<commit_message>
Adding new files- Combined Outflow 11452901- pTHg and SSC
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_SSC Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_SSC Model Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{315D1091-2995-46FB-9AE6-09152E2932C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{268390AE-22F0-494D-AA48-060231372198}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="887" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Model Results" sheetId="7" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Inlet" sheetId="3" r:id="rId3"/>
     <sheet name="Spillway" sheetId="4" r:id="rId4"/>
     <sheet name="Outlet" sheetId="5" r:id="rId5"/>
+    <sheet name="Combined Outlet" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1956" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="835">
   <si>
     <t>Model #</t>
   </si>
@@ -1962,6 +1963,573 @@
   </si>
   <si>
     <t>Outlet SSC (Using Combined Inst. Flow for Models Only)</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm1 &lt;- loadReg(SSC ~model(1), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(1), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 16</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.3403</t>
+  </si>
+  <si>
+    <t>(Intercept)   12.955     0.2560   50.61       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.696     0.1682   10.08       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8247</t>
+  </si>
+  <si>
+    <t>R-squared: 87.9 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 33.79 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0127</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2128</t>
+  </si>
+  <si>
+    <t>Est  6720 1640000 2410000 17700000 23700000 24500000 24500000</t>
+  </si>
+  <si>
+    <t>Obs 10300  207000 2370000 12700000 22400000 35500000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.747 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7502</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm2 &lt;- loadReg(SSC ~model(2), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(2), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm2</t>
+  </si>
+  <si>
+    <t>(Intercept)  12.6845     0.3600  35.239  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.6960     0.1674  10.132  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1169     0.1098   1.065  0.2472</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8169</t>
+  </si>
+  <si>
+    <t>R-squared: 88.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 35.13 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1273</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3877</t>
+  </si>
+  <si>
+    <t>Est  9970 1260000 1950000 21000000 30100000 31500000 31500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 25.37 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.6134</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm3 &lt;- loadReg(SSC ~model(3), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(3), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)  12.9165     0.2412  53.559   0.000</t>
+  </si>
+  <si>
+    <t>lnQ           1.8133     0.1721  10.539   0.000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.8518     0.4989  -1.707   0.072</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7255</t>
+  </si>
+  <si>
+    <t>R-squared: 90.11 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 37.03 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1789</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.0167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         VIF</t>
+  </si>
+  <si>
+    <t>lnQ     1.19</t>
+  </si>
+  <si>
+    <t>DECTIME 1.19</t>
+  </si>
+  <si>
+    <t>Est  7640 1220000 2730000 13800000 18400000 21200000 21200000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -7.293 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7568</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm4 &lt;- loadReg(SSC ~model(4), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(4), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  14.6844     2.5996  5.6486  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.6580     0.1856  8.9315  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.7971     2.1275 -0.8447  0.3364</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.8096     2.1137 -0.3830  0.6593</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8239</t>
+  </si>
+  <si>
+    <t>R-squared: 89.64 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 36.27 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0022</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2378</t>
+  </si>
+  <si>
+    <t>lnQ         1.219</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 8.461</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 9.077</t>
+  </si>
+  <si>
+    <t>Est  8570 1250000 2040000 15400000 33900000 38400000 38400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 19.97 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8052</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm5 &lt;- loadReg(SSC ~model(5), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(5), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept)  12.4546    0.32198  38.681  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.8545    0.15739  11.782  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1935    0.09903   1.954  0.0355</t>
+  </si>
+  <si>
+    <t>DECTIME      -1.1511    0.47752  -2.410  0.0120</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5963</t>
+  </si>
+  <si>
+    <t>R-squared: 92.5 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 41.45 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.149</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0428</t>
+  </si>
+  <si>
+    <t>lnQ     1.211</t>
+  </si>
+  <si>
+    <t>lnQ2    1.115</t>
+  </si>
+  <si>
+    <t>DECTIME 1.326</t>
+  </si>
+  <si>
+    <t>Est  9880 683000 2080000 16700000 25300000 30400000 30400000</t>
+  </si>
+  <si>
+    <t>Obs 10300 207000 2370000 12700000 22400000 35500000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 12.52 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.741</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm6 &lt;- loadReg(SSC ~model(6), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(6), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) 14.62151     2.6948  5.4258  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.67879     0.1977  8.4899  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.06238     0.1401  0.4453  0.5929</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -1.76163     2.2038 -0.7994  0.3419</t>
+  </si>
+  <si>
+    <t>cos.DECTIME -1.02324     2.2400 -0.4568  0.5835</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8829</t>
+  </si>
+  <si>
+    <t>R-squared: 89.82 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 36.56 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0186</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3343</t>
+  </si>
+  <si>
+    <t>lnQ         1.291</t>
+  </si>
+  <si>
+    <t>lnQ2        1.506</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 8.472</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 9.513</t>
+  </si>
+  <si>
+    <t>Est  9370 1210000 1800000 16800000 35900000 41700000 41700000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 27.43 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7047</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm7 &lt;- loadReg(SSC ~model(7), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(7), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)   16.442     2.1283   7.726  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ            1.839     0.1585  11.607  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME       -1.315     0.4516  -2.911  0.0025</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   -3.473     1.7666  -1.966  0.0282</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   -1.972     1.7067  -1.156  0.1757</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5078</t>
+  </si>
+  <si>
+    <t>R-squared: 94.15 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 45.41 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0925</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.2358</t>
+  </si>
+  <si>
+    <t>lnQ         1.442</t>
+  </si>
+  <si>
+    <t>DECTIME     1.393</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 9.466</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 9.603</t>
+  </si>
+  <si>
+    <t>Est  8230 780000 2690000  8680000 39500000 42800000 42800000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.19 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.6703</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm8 &lt;- loadReg(SSC ~model(8), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(8), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept)  16.5047     2.0356   8.108  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.9108     0.1597  11.967  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1495     0.1049   1.425  0.0855</t>
+  </si>
+  <si>
+    <t>DECTIME      -1.4743     0.4462  -3.304  0.0006</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -3.5913     1.6913  -2.123  0.0147</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -2.6257     1.6952  -1.549  0.0636</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.4643</t>
+  </si>
+  <si>
+    <t>R-squared: 95.13 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 48.36 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.9109</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.2849</t>
+  </si>
+  <si>
+    <t>lnQ          1.601</t>
+  </si>
+  <si>
+    <t>lnQ2         1.608</t>
+  </si>
+  <si>
+    <t>DECTIME      1.487</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  9.489</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 10.361</t>
+  </si>
+  <si>
+    <t>Est 10100 495000 2350000  9800000 44700000 51600000 51600000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 25.58 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.361</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm9 &lt;- loadReg(SSC ~model(9), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>In loadReg(SSC ~ model(9), data = SSC_Combined, flow = "Flow", dates = "Dates",  :</t>
+  </si>
+  <si>
+    <t>&gt; SSC_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept)  17.4620     1.9447  8.9794  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.3849     0.3397  4.0764  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.3509     0.1517  2.3130  0.0063</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.6255     0.6417 -0.9748  0.2051</t>
+  </si>
+  <si>
+    <t>DECTIME2    -14.6278     8.5298 -1.7149  0.0334</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.0518     2.1421 -0.4910  0.5154</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -2.0037     1.5932 -1.2577  0.1075</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.3888</t>
+  </si>
+  <si>
+    <t>R-squared: 96.33 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 52.89 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2059</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.1456</t>
+  </si>
+  <si>
+    <t>lnQ          8.653</t>
+  </si>
+  <si>
+    <t>lnQ2         4.011</t>
+  </si>
+  <si>
+    <t>DECTIME      3.671</t>
+  </si>
+  <si>
+    <t>DECTIME2    12.429</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 18.175</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 10.927</t>
+  </si>
+  <si>
+    <t>Est 10800 416000 2160000 10800000 44500000 54500000 54500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 28.29 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.2549</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 16; Period of record: 2016-01-24 to 2017-04-04</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2304,6 +2872,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2961,10 +3535,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>644</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="49"/>
       <c r="C1" s="9"/>
       <c r="K1" s="19" t="s">
         <v>248</v>
@@ -3008,17 +3582,17 @@
     </row>
     <row r="3" spans="1:34" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>643</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
       <c r="Y4" s="17" t="s">
         <v>253</v>
       </c>
@@ -3033,19 +3607,19 @@
       <c r="AH4" s="17"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="39" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="39"/>
+      <c r="L5" s="41"/>
       <c r="Y5" s="17" t="s">
         <v>254</v>
       </c>
@@ -3320,17 +3894,17 @@
       <c r="Y15" s="5"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
@@ -3343,19 +3917,19 @@
       <c r="AH17" s="9"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39" t="s">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="39"/>
+      <c r="L18" s="41"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
@@ -3627,32 +4201,32 @@
       <c r="Y28" s="5"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="39" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="39"/>
+      <c r="L31" s="41"/>
     </row>
     <row r="32" spans="1:34" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -3924,32 +4498,32 @@
       <c r="AA42" s="23"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="44"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="43"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="39" t="s">
+      <c r="B44" s="45"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="39"/>
+      <c r="L44" s="41"/>
     </row>
     <row r="45" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
@@ -4212,32 +4786,32 @@
       <c r="AA54" s="23"/>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="42"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="44"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B57" s="36"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="39" t="s">
+      <c r="B57" s="38"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="40"/>
+      <c r="K57" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L57" s="39"/>
+      <c r="L57" s="41"/>
     </row>
     <row r="58" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
@@ -4468,32 +5042,32 @@
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B70" s="40" t="s">
+      <c r="B70" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="41"/>
-      <c r="I70" s="41"/>
-      <c r="J70" s="42"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="43"/>
+      <c r="J70" s="44"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B71" s="36"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="39" t="s">
+      <c r="B71" s="38"/>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="39"/>
+      <c r="J71" s="40"/>
+      <c r="K71" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L71" s="39"/>
+      <c r="L71" s="41"/>
     </row>
     <row r="72" spans="1:14" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
@@ -4818,9 +5392,9 @@
   </sheetPr>
   <dimension ref="A1:AH68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4832,10 +5406,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="9"/>
       <c r="K1" s="19" t="s">
         <v>248</v>
@@ -4874,24 +5448,24 @@
       <c r="L2" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="52" t="s">
         <v>452</v>
       </c>
-      <c r="O2" s="51"/>
+      <c r="O2" s="53"/>
     </row>
     <row r="3" spans="1:34" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
       <c r="Y4" s="17" t="s">
         <v>253</v>
       </c>
@@ -4906,21 +5480,21 @@
       <c r="AH4" s="17"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="39" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="39"/>
+      <c r="L5" s="41"/>
       <c r="Y5" s="17" t="s">
         <v>254</v>
       </c>
@@ -4971,7 +5545,7 @@
       <c r="L6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="37" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="11" t="s">
@@ -5405,34 +5979,34 @@
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="42"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="38" t="s">
         <v>451</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="39"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
@@ -5471,7 +6045,7 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="37" t="s">
         <v>20</v>
       </c>
       <c r="N19" s="11" t="s">
@@ -5522,7 +6096,7 @@
       <c r="P20" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="AA20" s="23" t="s">
+      <c r="Z20" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5569,7 +6143,7 @@
       <c r="P21" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="AA21" s="23" t="s">
+      <c r="Z21" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5616,7 +6190,7 @@
       <c r="P22" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="AA22" s="23" t="s">
+      <c r="Z22" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5663,7 +6237,7 @@
       <c r="P23" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="AA23" s="23" t="s">
+      <c r="Z23" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5710,7 +6284,7 @@
       <c r="P24" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="AA24" s="23" t="s">
+      <c r="Z24" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5757,7 +6331,7 @@
       <c r="P25" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="AA25" s="23" t="s">
+      <c r="Z25" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5807,7 +6381,7 @@
       <c r="P26" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="AA26" s="23" t="s">
+      <c r="Z26" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5854,7 +6428,7 @@
       <c r="P27" s="22" t="s">
         <v>399</v>
       </c>
-      <c r="AA27" s="23" t="s">
+      <c r="Z27" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5901,7 +6475,7 @@
       <c r="P28" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="AA28" s="23" t="s">
+      <c r="Z28" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5911,34 +6485,34 @@
       <c r="AA29" s="23"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="42" t="s">
         <v>645</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="42"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="45" t="s">
         <v>642</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="39" t="s">
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="39"/>
+      <c r="L31" s="41"/>
     </row>
     <row r="32" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -5977,14 +6551,14 @@
       <c r="L32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="M32" s="37" t="s">
         <v>20</v>
       </c>
       <c r="N32" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>1</v>
       </c>
@@ -6027,11 +6601,11 @@
       <c r="P33" s="22" t="s">
         <v>454</v>
       </c>
-      <c r="AA33" s="23" t="s">
+      <c r="Z33" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>2</v>
       </c>
@@ -6074,11 +6648,11 @@
       <c r="P34" s="22" t="s">
         <v>476</v>
       </c>
-      <c r="AA34" s="23" t="s">
+      <c r="Z34" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>3</v>
       </c>
@@ -6121,11 +6695,11 @@
       <c r="P35" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="AA35" s="23" t="s">
+      <c r="Z35" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>4</v>
       </c>
@@ -6168,11 +6742,11 @@
       <c r="P36" s="22" t="s">
         <v>512</v>
       </c>
-      <c r="AA36" s="23" t="s">
+      <c r="Z36" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>5</v>
       </c>
@@ -6218,11 +6792,11 @@
       <c r="P37" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="AA37" s="23" t="s">
+      <c r="Z37" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>6</v>
       </c>
@@ -6265,11 +6839,11 @@
       <c r="P38" s="22" t="s">
         <v>551</v>
       </c>
-      <c r="AA38" s="23" t="s">
+      <c r="Z38" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>7</v>
       </c>
@@ -6312,11 +6886,11 @@
       <c r="P39" s="22" t="s">
         <v>573</v>
       </c>
-      <c r="AA39" s="23" t="s">
+      <c r="Z39" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>8</v>
       </c>
@@ -6359,11 +6933,11 @@
       <c r="P40" s="22" t="s">
         <v>594</v>
       </c>
-      <c r="AA40" s="23" t="s">
+      <c r="Z40" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>9</v>
       </c>
@@ -6406,39 +6980,41 @@
       <c r="P41" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="AA41" s="23" t="s">
+      <c r="Z41" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="40" t="s">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B43" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="42"/>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="36"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="38"/>
-      <c r="K44" s="39" t="s">
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="44"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B44" s="38" t="s">
+        <v>834</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="39"/>
-    </row>
-    <row r="45" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L44" s="41"/>
+    </row>
+    <row r="45" spans="1:26" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>0</v>
       </c>
@@ -6475,18 +7051,18 @@
       <c r="L45" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M45" s="13" t="s">
+      <c r="M45" s="37" t="s">
         <v>20</v>
       </c>
       <c r="N45" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A46" s="8">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A46" s="24">
         <v>1</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="24">
         <v>0</v>
       </c>
       <c r="C46" s="16" t="s">
@@ -6504,18 +7080,42 @@
       <c r="G46" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="H46" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="I46" s="24">
+        <v>87.9</v>
+      </c>
+      <c r="J46" s="24">
+        <v>0.21279999999999999</v>
+      </c>
+      <c r="K46" s="24">
+        <v>6.7469999999999999</v>
+      </c>
+      <c r="L46" s="36">
+        <v>0.75019999999999998</v>
+      </c>
+      <c r="M46" s="24"/>
+      <c r="N46" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P46" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="Z46" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>2</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="24">
         <v>0</v>
       </c>
-      <c r="C47" s="30"/>
+      <c r="C47" s="30">
+        <v>0.2472</v>
+      </c>
       <c r="D47" s="16" t="s">
         <v>14</v>
       </c>
@@ -6528,39 +7128,86 @@
       <c r="G47" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="15" t="s">
+      <c r="H47" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A48" s="8">
+      <c r="I47" s="36">
+        <v>88.87</v>
+      </c>
+      <c r="J47" s="36">
+        <v>0.38769999999999999</v>
+      </c>
+      <c r="K47" s="36">
+        <v>25.37</v>
+      </c>
+      <c r="L47" s="36">
+        <v>0.61339999999999995</v>
+      </c>
+      <c r="N47" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P47" s="22" t="s">
+        <v>667</v>
+      </c>
+      <c r="Z47" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="15">
         <v>3</v>
       </c>
       <c r="B48" s="15">
         <v>0</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="16" t="s">
+      <c r="C48" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="26">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I48" s="15">
+        <v>90.11</v>
+      </c>
+      <c r="J48" s="15">
+        <v>-1.67E-2</v>
+      </c>
+      <c r="K48" s="15">
+        <v>-7.2930000000000001</v>
+      </c>
+      <c r="L48" s="36">
+        <v>0.75680000000000003</v>
+      </c>
+      <c r="M48" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N48" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P48" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="Z48" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>4</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="24">
         <v>0</v>
       </c>
       <c r="C49" s="16" t="s">
@@ -6572,137 +7219,304 @@
       <c r="E49" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="15" t="s">
+      <c r="F49" s="24">
+        <v>0.33639999999999998</v>
+      </c>
+      <c r="G49" s="36">
+        <v>0.6593</v>
+      </c>
+      <c r="H49" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="8">
+      <c r="I49" s="36">
+        <v>89.64</v>
+      </c>
+      <c r="J49" s="36">
+        <v>0.23780000000000001</v>
+      </c>
+      <c r="K49" s="36">
+        <v>19.97</v>
+      </c>
+      <c r="L49" s="36">
+        <v>0.80520000000000003</v>
+      </c>
+      <c r="N49" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P49" s="22" t="s">
+        <v>702</v>
+      </c>
+      <c r="Z49" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A50" s="15">
         <v>5</v>
       </c>
       <c r="B50" s="15">
         <v>0</v>
       </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="16" t="s">
+      <c r="C50" s="15">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="D50" s="15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="33" t="s">
         <v>14</v>
       </c>
       <c r="H50" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I50" s="15">
+        <v>92.5</v>
+      </c>
+      <c r="J50" s="15">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="K50" s="15">
+        <v>12.52</v>
+      </c>
+      <c r="L50" s="36">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="M50" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N50" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P50" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="Z50" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>6</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="24">
         <v>0</v>
       </c>
-      <c r="C51" s="31"/>
+      <c r="C51" s="36">
+        <v>0.59289999999999998</v>
+      </c>
       <c r="D51" s="16" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="24"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="15" t="s">
+      <c r="F51" s="24">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="G51" s="36">
+        <v>0.58350000000000002</v>
+      </c>
+      <c r="H51" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I51" s="36">
+        <v>89.82</v>
+      </c>
+      <c r="J51" s="36">
+        <v>0.33429999999999999</v>
+      </c>
+      <c r="K51" s="36">
+        <v>27.43</v>
+      </c>
+      <c r="L51" s="36">
+        <v>0.70469999999999999</v>
+      </c>
+      <c r="N51" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P51" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="Z51" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>7</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="24">
         <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="24"/>
+      <c r="D52" s="24">
+        <v>2.5000000000000001E-3</v>
+      </c>
       <c r="E52" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="24"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="15" t="s">
+      <c r="F52" s="24">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="G52" s="36">
+        <v>0.1757</v>
+      </c>
+      <c r="H52" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I52" s="36">
+        <v>94.15</v>
+      </c>
+      <c r="J52" s="36">
+        <v>-0.23580000000000001</v>
+      </c>
+      <c r="K52" s="36">
+        <v>11.19</v>
+      </c>
+      <c r="L52" s="36">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="N52" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P52" s="22" t="s">
+        <v>764</v>
+      </c>
+      <c r="Z52" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>8</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="24">
         <v>0</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="24"/>
+      <c r="C53" s="36">
+        <v>8.5500000000000007E-2</v>
+      </c>
+      <c r="D53" s="24">
+        <v>5.9999999999999995E-4</v>
+      </c>
       <c r="E53" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="15" t="s">
+      <c r="F53" s="24">
+        <v>1.47E-2</v>
+      </c>
+      <c r="G53" s="24">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="H53" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I53" s="36">
+        <v>95.13</v>
+      </c>
+      <c r="J53" s="36">
+        <v>-0.28489999999999999</v>
+      </c>
+      <c r="K53" s="36">
+        <v>25.58</v>
+      </c>
+      <c r="L53" s="36">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="N53" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P53" s="22" t="s">
+        <v>786</v>
+      </c>
+      <c r="Z53" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>9</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="24">
         <v>0</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="15" t="s">
+      <c r="C54" s="36">
+        <v>6.3E-3</v>
+      </c>
+      <c r="D54" s="24">
+        <v>0.2051</v>
+      </c>
+      <c r="E54" s="24">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="F54" s="24">
+        <v>0.51539999999999997</v>
+      </c>
+      <c r="G54" s="24">
+        <v>0.1075</v>
+      </c>
+      <c r="H54" s="24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B57" s="40" t="s">
+      <c r="I54" s="36">
+        <v>96.33</v>
+      </c>
+      <c r="J54" s="36">
+        <v>-0.14560000000000001</v>
+      </c>
+      <c r="K54" s="36">
+        <v>28.29</v>
+      </c>
+      <c r="L54" s="36">
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="N54" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P54" s="22" t="s">
+        <v>810</v>
+      </c>
+      <c r="Z54" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B57" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="42"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B58" s="36"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="39" t="s">
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="44"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="39"/>
-    </row>
-    <row r="59" spans="1:14" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L58" s="41"/>
+    </row>
+    <row r="59" spans="1:26" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>0</v>
       </c>
@@ -6739,14 +7553,14 @@
       <c r="L59" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M59" s="13" t="s">
+      <c r="M59" s="37" t="s">
         <v>20</v>
       </c>
       <c r="N59" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>1</v>
       </c>
@@ -6772,7 +7586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>2</v>
       </c>
@@ -6796,7 +7610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>3</v>
       </c>
@@ -6820,7 +7634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>4</v>
       </c>
@@ -6842,7 +7656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>5</v>
       </c>
@@ -14392,4 +15206,2474 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1794C70D-1077-484D-B5F6-2A3A99F052C5}">
+  <dimension ref="A1:A528"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="4" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="4" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="3" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="3" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="4" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="5" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="4" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="2"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="2"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="2"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="4" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="5" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="4" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="2"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="2"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="3" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="3" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="3" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="3" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="3" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="3" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="3" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="3" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="3" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="3" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="3" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="3" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="2"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="3" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="2"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="3" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="3" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="3" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="2"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="4" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="5" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="4" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="2"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="2"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="2"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="2"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="2"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="3" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="3" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="3" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="3" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="3" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="2"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="3" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="3" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="3" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="3" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="3" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="2"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="3" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="3" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="3" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="3" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="2"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="3" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="2"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="3" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="3" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="3" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="2"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="4" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="5" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="4" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="2"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="2"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="3" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="3" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="2"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="2"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="2"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="3" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="3" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="3" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="3" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="3" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="3" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="3" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="2"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="3" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="3" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="3" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="2"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="3" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="3" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="3" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="3" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="3" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="2"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="2"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="3" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="3" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="3" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="6"/>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="6"/>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="7"/>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Combined Outflow 2016-2017 pTHg and SSC folders (deleted previous versions- # of observations changed from 16 to 34). Also added new files for wy 2016-2017 pTHg and SSC model stats, plus Combined Outflow Q and WQ Excel worksheet (several versions).
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_SSC Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_SSC Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{268390AE-22F0-494D-AA48-060231372198}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5FCA5DCD-860A-4A8D-B4FD-5D12FF57130A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="887" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="Inlet" sheetId="3" r:id="rId3"/>
     <sheet name="Spillway" sheetId="4" r:id="rId4"/>
     <sheet name="Outlet" sheetId="5" r:id="rId5"/>
-    <sheet name="Combined Outlet" sheetId="8" r:id="rId6"/>
+    <sheet name="Combined Outlet" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="837">
   <si>
     <t>Model #</t>
   </si>
@@ -1974,57 +1974,6 @@
     <t>&gt; SSC_Combinedm1</t>
   </si>
   <si>
-    <t xml:space="preserve">           Number of Observations: 16</t>
-  </si>
-  <si>
-    <t>Number of Uncensored Observations: 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           Center of Decimal Time: 2016.652</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  Center of ln(Q): 7.3403</t>
-  </si>
-  <si>
-    <t>(Intercept)   12.955     0.2560   50.61       0</t>
-  </si>
-  <si>
-    <t>lnQ            1.696     0.1682   10.08       0</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.8247</t>
-  </si>
-  <si>
-    <t>R-squared: 87.9 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 33.79 on 1 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0127</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2128</t>
-  </si>
-  <si>
-    <t>Est  6720 1640000 2410000 17700000 23700000 24500000 24500000</t>
-  </si>
-  <si>
-    <t>Obs 10300  207000 2370000 12700000 22400000 35500000 35500000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 6.747 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.7502</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm2 &lt;- loadReg(SSC ~model(2), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2034,45 +1983,6 @@
     <t>&gt; SSC_Combinedm2</t>
   </si>
   <si>
-    <t>(Intercept)  12.6845     0.3600  35.239  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.6960     0.1674  10.132  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2          0.1169     0.1098   1.065  0.2472</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.8169</t>
-  </si>
-  <si>
-    <t>R-squared: 88.87 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 35.13 on 2 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9569</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.1273</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.3877</t>
-  </si>
-  <si>
-    <t>Est  9970 1260000 1950000 21000000 30100000 31500000 31500000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 25.37 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.6134</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm3 &lt;- loadReg(SSC ~model(3), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2082,54 +1992,6 @@
     <t>&gt; SSC_Combinedm3</t>
   </si>
   <si>
-    <t>(Intercept)  12.9165     0.2412  53.559   0.000</t>
-  </si>
-  <si>
-    <t>lnQ           1.8133     0.1721  10.539   0.000</t>
-  </si>
-  <si>
-    <t>DECTIME      -0.8518     0.4989  -1.707   0.072</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.7255</t>
-  </si>
-  <si>
-    <t>R-squared: 90.11 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 37.03 on 2 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.962</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.1789</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: -0.0167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         VIF</t>
-  </si>
-  <si>
-    <t>lnQ     1.19</t>
-  </si>
-  <si>
-    <t>DECTIME 1.19</t>
-  </si>
-  <si>
-    <t>Est  7640 1220000 2730000 13800000 18400000 21200000 21200000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: -7.293 percent</t>
-  </si>
-  <si>
-    <t>PLR: 0.9271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.7568</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm4 &lt;- loadReg(SSC ~model(4), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2139,57 +2001,12 @@
     <t>&gt; SSC_Combinedm4</t>
   </si>
   <si>
-    <t>(Intercept)  14.6844     2.5996  5.6486  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.6580     0.1856  8.9315  0.0000</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  -1.7971     2.1275 -0.8447  0.3364</t>
-  </si>
-  <si>
-    <t>cos.DECTIME  -0.8096     2.1137 -0.3830  0.6593</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.8239</t>
-  </si>
-  <si>
-    <t>R-squared: 89.64 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 36.27 on 3 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0022</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.2378</t>
-  </si>
-  <si>
     <t>lnQ         1.219</t>
   </si>
   <si>
-    <t>sin.DECTIME 8.461</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 9.077</t>
-  </si>
-  <si>
-    <t>Est  8570 1250000 2040000 15400000 33900000 38400000 38400000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 19.97 percent</t>
-  </si>
-  <si>
     <t>PLR: 1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">  E: 0.8052</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm5 &lt;- loadReg(SSC ~model(5), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2199,57 +2016,9 @@
     <t>&gt; SSC_Combinedm5</t>
   </si>
   <si>
-    <t>(Intercept)  12.4546    0.32198  38.681  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.8545    0.15739  11.782  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2          0.1935    0.09903   1.954  0.0355</t>
-  </si>
-  <si>
-    <t>DECTIME      -1.1511    0.47752  -2.410  0.0120</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.5963</t>
-  </si>
-  <si>
-    <t>R-squared: 92.5 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 41.45 on 3 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.149</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.0428</t>
-  </si>
-  <si>
     <t>lnQ     1.211</t>
   </si>
   <si>
-    <t>lnQ2    1.115</t>
-  </si>
-  <si>
-    <t>DECTIME 1.326</t>
-  </si>
-  <si>
-    <t>Est  9880 683000 2080000 16700000 25300000 30400000 30400000</t>
-  </si>
-  <si>
-    <t>Obs 10300 207000 2370000 12700000 22400000 35500000 35500000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 12.52 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.741</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm6 &lt;- loadReg(SSC ~model(6), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2259,63 +2028,6 @@
     <t>&gt; SSC_Combinedm6</t>
   </si>
   <si>
-    <t>(Intercept) 14.62151     2.6948  5.4258  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ          1.67879     0.1977  8.4899  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2         0.06238     0.1401  0.4453  0.5929</t>
-  </si>
-  <si>
-    <t>sin.DECTIME -1.76163     2.2038 -0.7994  0.3419</t>
-  </si>
-  <si>
-    <t>cos.DECTIME -1.02324     2.2400 -0.4568  0.5835</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.8829</t>
-  </si>
-  <si>
-    <t>R-squared: 89.82 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 36.56 on 4 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0186</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: 0.3343</t>
-  </si>
-  <si>
-    <t>lnQ         1.291</t>
-  </si>
-  <si>
-    <t>lnQ2        1.506</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 8.472</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 9.513</t>
-  </si>
-  <si>
-    <t>Est  9370 1210000 1800000 16800000 35900000 41700000 41700000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 27.43 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.274</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.7047</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm7 &lt;- loadReg(SSC ~model(7), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2325,63 +2037,6 @@
     <t>&gt; SSC_Combinedm7</t>
   </si>
   <si>
-    <t>(Intercept)   16.442     2.1283   7.726  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ            1.839     0.1585  11.607  0.0000</t>
-  </si>
-  <si>
-    <t>DECTIME       -1.315     0.4516  -2.911  0.0025</t>
-  </si>
-  <si>
-    <t>sin.DECTIME   -3.473     1.7666  -1.966  0.0282</t>
-  </si>
-  <si>
-    <t>cos.DECTIME   -1.972     1.7067  -1.156  0.1757</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.5078</t>
-  </si>
-  <si>
-    <t>R-squared: 94.15 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 45.41 on 4 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.952</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.0925</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: -0.2358</t>
-  </si>
-  <si>
-    <t>lnQ         1.442</t>
-  </si>
-  <si>
-    <t>DECTIME     1.393</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 9.466</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 9.603</t>
-  </si>
-  <si>
-    <t>Est  8230 780000 2690000  8680000 39500000 42800000 42800000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 11.19 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.6703</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm8 &lt;- loadReg(SSC ~model(8), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2391,69 +2046,6 @@
     <t>&gt; SSC_Combinedm8</t>
   </si>
   <si>
-    <t>(Intercept)  16.5047     2.0356   8.108  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.9108     0.1597  11.967  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2          0.1495     0.1049   1.425  0.0855</t>
-  </si>
-  <si>
-    <t>DECTIME      -1.4743     0.4462  -3.304  0.0006</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  -3.5913     1.6913  -2.123  0.0147</t>
-  </si>
-  <si>
-    <t>cos.DECTIME  -2.6257     1.6952  -1.549  0.0636</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.4643</t>
-  </si>
-  <si>
-    <t>R-squared: 95.13 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 48.36 on 5 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  r = 0.9896</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.9109</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: -0.2849</t>
-  </si>
-  <si>
-    <t>lnQ          1.601</t>
-  </si>
-  <si>
-    <t>lnQ2         1.608</t>
-  </si>
-  <si>
-    <t>DECTIME      1.487</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  9.489</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 10.361</t>
-  </si>
-  <si>
-    <t>Est 10100 495000 2350000  9800000 44700000 51600000 51600000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 25.58 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.361</t>
-  </si>
-  <si>
     <t>&gt; SSC_Combinedm9 &lt;- loadReg(SSC ~model(9), data = SSC_Combined , flow="Flow", dates = "Dates" ,conc.units="mg/L" , station = "CCSB-Yolo")</t>
   </si>
   <si>
@@ -2463,73 +2055,487 @@
     <t>&gt; SSC_Combinedm9</t>
   </si>
   <si>
-    <t>(Intercept)  17.4620     1.9447  8.9794  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ           1.3849     0.3397  4.0764  0.0000</t>
-  </si>
-  <si>
-    <t>lnQ2          0.3509     0.1517  2.3130  0.0063</t>
-  </si>
-  <si>
-    <t>DECTIME      -0.6255     0.6417 -0.9748  0.2051</t>
-  </si>
-  <si>
-    <t>DECTIME2    -14.6278     8.5298 -1.7149  0.0334</t>
-  </si>
-  <si>
-    <t>sin.DECTIME  -1.0518     2.1421 -0.4910  0.5154</t>
-  </si>
-  <si>
-    <t>cos.DECTIME  -2.0037     1.5932 -1.2577  0.1075</t>
-  </si>
-  <si>
-    <t>Residual variance: 0.3888</t>
-  </si>
-  <si>
-    <t>R-squared: 96.33 percent</t>
-  </si>
-  <si>
-    <t>G-squared: 52.89 on 6 degrees of freedom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  p-value = 0.2059</t>
-  </si>
-  <si>
-    <t>Serial Correlation of Residuals: -0.1456</t>
-  </si>
-  <si>
-    <t>lnQ          8.653</t>
-  </si>
-  <si>
-    <t>lnQ2         4.011</t>
-  </si>
-  <si>
-    <t>DECTIME      3.671</t>
-  </si>
-  <si>
-    <t>DECTIME2    12.429</t>
-  </si>
-  <si>
-    <t>sin.DECTIME 18.175</t>
-  </si>
-  <si>
-    <t>cos.DECTIME 10.927</t>
-  </si>
-  <si>
-    <t>Est 10800 416000 2160000 10800000 44500000 54500000 54500000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bp: 28.29 percent</t>
-  </si>
-  <si>
-    <t>PLR: 1.283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  E: 0.2549</t>
-  </si>
-  <si>
-    <t>Number of Uncensored Observations: 16; Period of record: 2016-01-24 to 2017-04-04</t>
+    <t xml:space="preserve">           Number of Observations: 34</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0699</t>
+  </si>
+  <si>
+    <t>(Intercept)   12.933     0.1783   72.52       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.484     0.1072   13.84       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 1.059</t>
+  </si>
+  <si>
+    <t>R-squared: 85.68 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 66.08 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1683</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Min    25%     50%     75%      90%      95%      Max</t>
+  </si>
+  <si>
+    <t>Est 7060 153000 2600000 9020000 19800000 24900000 25600000</t>
+  </si>
+  <si>
+    <t>Obs 2710  90200 1020000 6210000 14900000 22400000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 20.86 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7727</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.84551    0.28339 45.3276  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.48372    0.10866 13.6542  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.03161    0.07891  0.4006  0.6752</t>
+  </si>
+  <si>
+    <t>Residual variance: 1.088</t>
+  </si>
+  <si>
+    <t>R-squared: 85.75 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 66.25 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1229</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.556</t>
+  </si>
+  <si>
+    <t>Est 7710 145000 2450000 9210000 21200000 27000000 27900000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 26.87 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7363</t>
+  </si>
+  <si>
+    <t>(Intercept)  12.9481     0.1688  76.710  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.5857     0.1116  14.208  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.8575     0.3920  -2.187  0.0272</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9472</t>
+  </si>
+  <si>
+    <t>R-squared: 87.59 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 70.96 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7777</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4916</t>
+  </si>
+  <si>
+    <t>DECTIME 1.211</t>
+  </si>
+  <si>
+    <t>Est 6400 207000 2230000 7190000 15800000 19700000 22500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 6.123 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8069</t>
+  </si>
+  <si>
+    <t>(Intercept)  11.3910     1.0634 10.7117  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4093     0.1140 12.3668  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.8889     0.9219  0.9643  0.3083</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.6311     0.9040  1.8043  0.0613</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9813</t>
+  </si>
+  <si>
+    <t>R-squared: 87.56 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 70.87 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9686</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0536</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4498</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.817</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.874</t>
+  </si>
+  <si>
+    <t>Est 10200 100000 1800000 10100000 21200000 23800000 25100000</t>
+  </si>
+  <si>
+    <t>Obs  2710  90200 1020000  6210000 14900000 22400000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 22.67 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7382</t>
+  </si>
+  <si>
+    <t>(Intercept) 12.68192    0.27006  46.960  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.60659    0.11183  14.366  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.09734    0.07755   1.255  0.1871</t>
+  </si>
+  <si>
+    <t>DECTIME     -1.03309    0.41286  -2.502  0.0111</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.9299</t>
+  </si>
+  <si>
+    <t>R-squared: 88.21 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 72.7 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2934</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5054</t>
+  </si>
+  <si>
+    <t>lnQ     1.239</t>
+  </si>
+  <si>
+    <t>lnQ2    1.130</t>
+  </si>
+  <si>
+    <t>DECTIME 1.368</t>
+  </si>
+  <si>
+    <t>Est 8540 180000 1750000 7070000 19000000 25100000 29400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 19.96 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7823</t>
+  </si>
+  <si>
+    <t>(Intercept)  11.4502    1.14672  9.9852  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4102    0.11598 12.1585  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         -0.0135    0.08719 -0.1549  0.8668</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.8480    0.97369  0.8710  0.3488</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.6318    0.91909  1.7754  0.0611</t>
+  </si>
+  <si>
+    <t>Residual variance: 1.014</t>
+  </si>
+  <si>
+    <t>R-squared: 87.57 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 70.9 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0459</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4404</t>
+  </si>
+  <si>
+    <t>lnQ         1.222</t>
+  </si>
+  <si>
+    <t>lnQ2        1.309</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.119</t>
+  </si>
+  <si>
+    <t>Est 9070 102000 1840000 10300000 20300000 21800000 24400000</t>
+  </si>
+  <si>
+    <t>Obs 2710  90200 1020000  6210000 14900000 22400000 35500000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 20.38 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7638</t>
+  </si>
+  <si>
+    <t>(Intercept)  13.3793     1.2726 10.5131  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.6437     0.1420 11.5729  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -1.2265     0.4981 -2.4623  0.0111</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.9947     1.1456 -0.8683  0.3502</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   0.1818     1.0226  0.1778  0.8474</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8396</t>
+  </si>
+  <si>
+    <t>R-squared: 89.71 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.33 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1151</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4165</t>
+  </si>
+  <si>
+    <t>lnQ         2.213</t>
+  </si>
+  <si>
+    <t>DECTIME     2.206</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.888</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.793</t>
+  </si>
+  <si>
+    <t>Est 8370 114000 2090000 8460000 14900000 28100000 31900000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.83 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8967</t>
+  </si>
+  <si>
+    <t>(Intercept) 13.31486    1.30565 10.1979  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.64919    0.14509 11.3667  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.02861    0.08238  0.3473  0.7022</t>
+  </si>
+  <si>
+    <t>DECTIME     -1.26405    0.51727 -2.4437  0.0104</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.96581    1.16630 -0.8281  0.3644</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.13590    1.04681  0.1298  0.8863</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8658</t>
+  </si>
+  <si>
+    <t>R-squared: 89.76 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.47 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1062</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4316</t>
+  </si>
+  <si>
+    <t>lnQ         2.240</t>
+  </si>
+  <si>
+    <t>lnQ2        1.369</t>
+  </si>
+  <si>
+    <t>DECTIME     2.307</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.924</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.887</t>
+  </si>
+  <si>
+    <t>Est 8610 116000 1960000 8390000 15500000 29600000 33900000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 15.66 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8821</t>
+  </si>
+  <si>
+    <t>(Intercept) 13.24776    1.32460 10.0013  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ          1.58201    0.18222  8.6817  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.04034    0.08541  0.4723  0.5969</t>
+  </si>
+  <si>
+    <t>DECTIME     -1.08175    0.59964 -1.8040  0.0492</t>
+  </si>
+  <si>
+    <t>DECTIME2    -1.72756    2.77921 -0.6216  0.4870</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.47645    1.41793 -0.3360  0.7064</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.37359    1.12542  0.3320  0.7098</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8852</t>
+  </si>
+  <si>
+    <t>R-squared: 89.9 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.96 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1885</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4246</t>
+  </si>
+  <si>
+    <t>lnQ          3.456</t>
+  </si>
+  <si>
+    <t>lnQ2         1.440</t>
+  </si>
+  <si>
+    <t>DECTIME      3.033</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.943</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 10.009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  6.656</t>
+  </si>
+  <si>
+    <t>Est 6010 134000 2060000 8450000 15600000 28100000 32400000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 14.93 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8847</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34; Period of record: 2016-01-20 to 2017-04-26</t>
   </si>
 </sst>
 </file>
@@ -2872,20 +2878,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2908,10 +2902,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2920,17 +2932,71 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3535,10 +3601,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="45" t="s">
         <v>644</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="9"/>
       <c r="K1" s="19" t="s">
         <v>248</v>
@@ -3582,17 +3648,17 @@
     </row>
     <row r="3" spans="1:34" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>643</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
       <c r="Y4" s="17" t="s">
         <v>253</v>
       </c>
@@ -3607,19 +3673,19 @@
       <c r="AH4" s="17"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="44"/>
       <c r="Y5" s="17" t="s">
         <v>254</v>
       </c>
@@ -3894,17 +3960,17 @@
       <c r="Y15" s="5"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
@@ -3917,19 +3983,19 @@
       <c r="AH17" s="9"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41" t="s">
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="41"/>
+      <c r="L18" s="44"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
@@ -4201,32 +4267,32 @@
       <c r="Y28" s="5"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="44"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="41" t="s">
+      <c r="B31" s="47"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="41"/>
+      <c r="L31" s="44"/>
     </row>
     <row r="32" spans="1:34" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -4498,32 +4564,32 @@
       <c r="AA42" s="23"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="44"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="41" t="s">
+      <c r="B44" s="41"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="41"/>
+      <c r="L44" s="44"/>
     </row>
     <row r="45" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
@@ -4786,32 +4852,32 @@
       <c r="AA54" s="23"/>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="44"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="40"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B57" s="38"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="41" t="s">
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L57" s="41"/>
+      <c r="L57" s="44"/>
     </row>
     <row r="58" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
@@ -5042,32 +5108,32 @@
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B70" s="42" t="s">
+      <c r="B70" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="43"/>
-      <c r="J70" s="44"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="40"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B71" s="38"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="40"/>
-      <c r="K71" s="41" t="s">
+      <c r="B71" s="47"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="48"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L71" s="41"/>
+      <c r="L71" s="44"/>
     </row>
     <row r="72" spans="1:14" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
@@ -5299,6 +5365,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B70:J70"/>
+    <mergeCell ref="B71:J71"/>
+    <mergeCell ref="K71:L71"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="K44:L44"/>
@@ -5313,71 +5384,66 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="B31:J31"/>
     <mergeCell ref="K31:L31"/>
-    <mergeCell ref="B57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B70:J70"/>
-    <mergeCell ref="B71:J71"/>
-    <mergeCell ref="K71:L71"/>
   </mergeCells>
   <conditionalFormatting sqref="L20:L28 L73:L81 L46:L54 L33:L41 L103:L1048576">
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59:L67">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K28 K46:K54 K73:K1048576 K33:K42 K59:K70 K30">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74 D75 C77:C78 D77 C80:C81 D79:D81 E81 F76:G76 F78:G81 C60 D61 C63:C64 D63 C66:C67 D65:D67 E67 F62:G62 F64:G67">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L15">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K15">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54 C34 D35 C37:C38 D37 C40:C41 D39:D41 E41 F36:G36 F38:G41 C21 D22 C24:C25 D24 C27:C28 D26:D28 E28 F23:G23 F25:G28 C8 D9 C11:C12 D11 C14:C15 D13:D15 E15 F10:G10 F12:G15">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5393,7 +5459,7 @@
   <dimension ref="A1:AH68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
@@ -5406,10 +5472,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="53"/>
       <c r="C1" s="9"/>
       <c r="K1" s="19" t="s">
         <v>248</v>
@@ -5448,24 +5514,24 @@
       <c r="L2" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="50" t="s">
         <v>452</v>
       </c>
-      <c r="O2" s="53"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:34" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
       <c r="Y4" s="17" t="s">
         <v>253</v>
       </c>
@@ -5480,21 +5546,21 @@
       <c r="AH4" s="17"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="47" t="s">
         <v>250</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="44"/>
       <c r="Y5" s="17" t="s">
         <v>254</v>
       </c>
@@ -5545,7 +5611,7 @@
       <c r="L6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="36" t="s">
         <v>20</v>
       </c>
       <c r="N6" s="11" t="s">
@@ -5979,34 +6045,34 @@
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="47" t="s">
         <v>451</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41" t="s">
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="41"/>
+      <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
@@ -6045,7 +6111,7 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="37" t="s">
+      <c r="M19" s="36" t="s">
         <v>20</v>
       </c>
       <c r="N19" s="11" t="s">
@@ -6485,34 +6551,34 @@
       <c r="AA29" s="23"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="38" t="s">
         <v>645</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="44"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="41" t="s">
         <v>642</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="41" t="s">
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="41"/>
+      <c r="L31" s="44"/>
     </row>
     <row r="32" spans="1:27" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
@@ -6551,7 +6617,7 @@
       <c r="L32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M32" s="37" t="s">
+      <c r="M32" s="36" t="s">
         <v>20</v>
       </c>
       <c r="N32" s="11" t="s">
@@ -6985,34 +7051,34 @@
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="44"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B44" s="38" t="s">
-        <v>834</v>
-      </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="41" t="s">
+      <c r="B44" s="47" t="s">
+        <v>836</v>
+      </c>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="41"/>
+      <c r="L44" s="44"/>
     </row>
     <row r="45" spans="1:26" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
@@ -7051,7 +7117,7 @@
       <c r="L45" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M45" s="37" t="s">
+      <c r="M45" s="36" t="s">
         <v>20</v>
       </c>
       <c r="N45" s="11" t="s">
@@ -7059,7 +7125,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="24">
+      <c r="A46" s="37">
         <v>1</v>
       </c>
       <c r="B46" s="24">
@@ -7083,19 +7149,19 @@
       <c r="H46" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="24">
-        <v>87.9</v>
-      </c>
-      <c r="J46" s="24">
-        <v>0.21279999999999999</v>
-      </c>
-      <c r="K46" s="24">
-        <v>6.7469999999999999</v>
-      </c>
-      <c r="L46" s="36">
-        <v>0.75019999999999998</v>
-      </c>
-      <c r="M46" s="24"/>
+      <c r="I46" s="37">
+        <v>85.68</v>
+      </c>
+      <c r="J46" s="37">
+        <v>0.54159999999999997</v>
+      </c>
+      <c r="K46" s="37">
+        <v>20.86</v>
+      </c>
+      <c r="L46" s="37">
+        <v>0.77270000000000005</v>
+      </c>
+      <c r="M46" s="37"/>
       <c r="N46" s="22" t="s">
         <v>16</v>
       </c>
@@ -7107,14 +7173,14 @@
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="8">
+      <c r="A47" s="37">
         <v>2</v>
       </c>
       <c r="B47" s="24">
         <v>0</v>
       </c>
       <c r="C47" s="30">
-        <v>0.2472</v>
+        <v>0.67520000000000002</v>
       </c>
       <c r="D47" s="16" t="s">
         <v>14</v>
@@ -7131,23 +7197,24 @@
       <c r="H47" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="36">
-        <v>88.87</v>
-      </c>
-      <c r="J47" s="36">
-        <v>0.38769999999999999</v>
-      </c>
-      <c r="K47" s="36">
-        <v>25.37</v>
-      </c>
-      <c r="L47" s="36">
-        <v>0.61339999999999995</v>
-      </c>
+      <c r="I47" s="37">
+        <v>85.75</v>
+      </c>
+      <c r="J47" s="37">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="K47" s="37">
+        <v>26.87</v>
+      </c>
+      <c r="L47" s="37">
+        <v>0.73629999999999995</v>
+      </c>
+      <c r="M47" s="37"/>
       <c r="N47" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P47" s="22" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
       <c r="Z47" s="23" t="s">
         <v>18</v>
@@ -7164,7 +7231,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="26">
-        <v>7.1999999999999995E-2</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="E48" s="33" t="s">
         <v>14</v>
@@ -7179,16 +7246,16 @@
         <v>7</v>
       </c>
       <c r="I48" s="15">
-        <v>90.11</v>
+        <v>87.59</v>
       </c>
       <c r="J48" s="15">
-        <v>-1.67E-2</v>
+        <v>0.49159999999999998</v>
       </c>
       <c r="K48" s="15">
-        <v>-7.2930000000000001</v>
-      </c>
-      <c r="L48" s="36">
-        <v>0.75680000000000003</v>
+        <v>6.1230000000000002</v>
+      </c>
+      <c r="L48" s="37">
+        <v>0.80689999999999995</v>
       </c>
       <c r="M48" s="15" t="s">
         <v>8</v>
@@ -7197,14 +7264,14 @@
         <v>16</v>
       </c>
       <c r="P48" s="22" t="s">
-        <v>683</v>
+        <v>653</v>
       </c>
       <c r="Z48" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="8">
+      <c r="A49" s="37">
         <v>4</v>
       </c>
       <c r="B49" s="24">
@@ -7220,95 +7287,94 @@
         <v>14</v>
       </c>
       <c r="F49" s="24">
-        <v>0.33639999999999998</v>
-      </c>
-      <c r="G49" s="36">
-        <v>0.6593</v>
+        <v>0.30830000000000002</v>
+      </c>
+      <c r="G49" s="37">
+        <v>6.13E-2</v>
       </c>
       <c r="H49" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="36">
-        <v>89.64</v>
-      </c>
-      <c r="J49" s="36">
-        <v>0.23780000000000001</v>
-      </c>
-      <c r="K49" s="36">
-        <v>19.97</v>
-      </c>
-      <c r="L49" s="36">
-        <v>0.80520000000000003</v>
-      </c>
+      <c r="I49" s="37">
+        <v>87.56</v>
+      </c>
+      <c r="J49" s="37">
+        <v>0.44979999999999998</v>
+      </c>
+      <c r="K49" s="37">
+        <v>22.67</v>
+      </c>
+      <c r="L49" s="37">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="M49" s="37"/>
       <c r="N49" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P49" s="22" t="s">
-        <v>702</v>
+        <v>656</v>
       </c>
       <c r="Z49" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50" s="15">
+      <c r="A50" s="37">
         <v>5</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="24">
         <v>0</v>
       </c>
-      <c r="C50" s="15">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="D50" s="15">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E50" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50" s="15" t="s">
+      <c r="C50" s="37">
+        <v>0.18709999999999999</v>
+      </c>
+      <c r="D50" s="37">
+        <v>1.11E-2</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="15">
-        <v>92.5</v>
-      </c>
-      <c r="J50" s="15">
-        <v>4.2799999999999998E-2</v>
-      </c>
-      <c r="K50" s="15">
-        <v>12.52</v>
-      </c>
-      <c r="L50" s="36">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="M50" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="I50" s="37">
+        <v>88.21</v>
+      </c>
+      <c r="J50" s="37">
+        <v>0.50539999999999996</v>
+      </c>
+      <c r="K50" s="37">
+        <v>19.96</v>
+      </c>
+      <c r="L50" s="37">
+        <v>0.7823</v>
+      </c>
+      <c r="M50" s="37"/>
       <c r="N50" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P50" s="22" t="s">
-        <v>722</v>
+        <v>661</v>
       </c>
       <c r="Z50" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="8">
+      <c r="A51" s="37">
         <v>6</v>
       </c>
       <c r="B51" s="24">
         <v>0</v>
       </c>
-      <c r="C51" s="36">
-        <v>0.59289999999999998</v>
+      <c r="C51" s="37">
+        <v>0.86680000000000001</v>
       </c>
       <c r="D51" s="16" t="s">
         <v>14</v>
@@ -7317,38 +7383,39 @@
         <v>14</v>
       </c>
       <c r="F51" s="24">
-        <v>0.34189999999999998</v>
-      </c>
-      <c r="G51" s="36">
-        <v>0.58350000000000002</v>
+        <v>0.3488</v>
+      </c>
+      <c r="G51" s="37">
+        <v>6.1100000000000002E-2</v>
       </c>
       <c r="H51" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="36">
-        <v>89.82</v>
-      </c>
-      <c r="J51" s="36">
-        <v>0.33429999999999999</v>
-      </c>
-      <c r="K51" s="36">
-        <v>27.43</v>
-      </c>
-      <c r="L51" s="36">
-        <v>0.70469999999999999</v>
-      </c>
+      <c r="I51" s="37">
+        <v>87.57</v>
+      </c>
+      <c r="J51" s="37">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="K51" s="37">
+        <v>20.38</v>
+      </c>
+      <c r="L51" s="37">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="M51" s="37"/>
       <c r="N51" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P51" s="22" t="s">
-        <v>742</v>
+        <v>665</v>
       </c>
       <c r="Z51" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="8">
+      <c r="A52" s="37">
         <v>7</v>
       </c>
       <c r="B52" s="24">
@@ -7358,163 +7425,166 @@
         <v>14</v>
       </c>
       <c r="D52" s="24">
-        <v>2.5000000000000001E-3</v>
+        <v>1.11E-2</v>
       </c>
       <c r="E52" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F52" s="24">
-        <v>2.8199999999999999E-2</v>
-      </c>
-      <c r="G52" s="36">
-        <v>0.1757</v>
+        <v>0.35020000000000001</v>
+      </c>
+      <c r="G52" s="37">
+        <v>0.84740000000000004</v>
       </c>
       <c r="H52" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="36">
-        <v>94.15</v>
-      </c>
-      <c r="J52" s="36">
-        <v>-0.23580000000000001</v>
-      </c>
-      <c r="K52" s="36">
-        <v>11.19</v>
-      </c>
-      <c r="L52" s="36">
-        <v>0.67030000000000001</v>
-      </c>
+      <c r="I52" s="37">
+        <v>89.71</v>
+      </c>
+      <c r="J52" s="37">
+        <v>0.41649999999999998</v>
+      </c>
+      <c r="K52" s="37">
+        <v>11.83</v>
+      </c>
+      <c r="L52" s="37">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="M52" s="37"/>
       <c r="N52" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P52" s="22" t="s">
-        <v>764</v>
+        <v>668</v>
       </c>
       <c r="Z52" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="8">
+      <c r="A53" s="37">
         <v>8</v>
       </c>
       <c r="B53" s="24">
         <v>0</v>
       </c>
-      <c r="C53" s="36">
-        <v>8.5500000000000007E-2</v>
+      <c r="C53" s="37">
+        <v>0.70220000000000005</v>
       </c>
       <c r="D53" s="24">
-        <v>5.9999999999999995E-4</v>
+        <v>1.04E-2</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F53" s="24">
-        <v>1.47E-2</v>
+        <v>0.3644</v>
       </c>
       <c r="G53" s="24">
-        <v>6.3600000000000004E-2</v>
+        <v>0.88629999999999998</v>
       </c>
       <c r="H53" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="36">
-        <v>95.13</v>
-      </c>
-      <c r="J53" s="36">
-        <v>-0.28489999999999999</v>
-      </c>
-      <c r="K53" s="36">
-        <v>25.58</v>
-      </c>
-      <c r="L53" s="36">
-        <v>0.36099999999999999</v>
-      </c>
+      <c r="I53" s="37">
+        <v>89.76</v>
+      </c>
+      <c r="J53" s="37">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="K53" s="37">
+        <v>15.66</v>
+      </c>
+      <c r="L53" s="37">
+        <v>0.8821</v>
+      </c>
+      <c r="M53" s="37"/>
       <c r="N53" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P53" s="22" t="s">
-        <v>786</v>
+        <v>671</v>
       </c>
       <c r="Z53" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="8">
+      <c r="A54" s="37">
         <v>9</v>
       </c>
       <c r="B54" s="24">
         <v>0</v>
       </c>
-      <c r="C54" s="36">
-        <v>6.3E-3</v>
+      <c r="C54" s="37">
+        <v>0.59689999999999999</v>
       </c>
       <c r="D54" s="24">
-        <v>0.2051</v>
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="E54" s="24">
-        <v>3.3399999999999999E-2</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="F54" s="24">
-        <v>0.51539999999999997</v>
+        <v>0.70640000000000003</v>
       </c>
       <c r="G54" s="24">
-        <v>0.1075</v>
+        <v>0.70979999999999999</v>
       </c>
       <c r="H54" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="36">
-        <v>96.33</v>
-      </c>
-      <c r="J54" s="36">
-        <v>-0.14560000000000001</v>
-      </c>
-      <c r="K54" s="36">
-        <v>28.29</v>
-      </c>
-      <c r="L54" s="36">
-        <v>0.25490000000000002</v>
-      </c>
+      <c r="I54" s="37">
+        <v>89.9</v>
+      </c>
+      <c r="J54" s="37">
+        <v>0.42459999999999998</v>
+      </c>
+      <c r="K54" s="37">
+        <v>14.93</v>
+      </c>
+      <c r="L54" s="37">
+        <v>0.88470000000000004</v>
+      </c>
+      <c r="M54" s="37"/>
       <c r="N54" s="22" t="s">
         <v>16</v>
       </c>
       <c r="P54" s="22" t="s">
-        <v>810</v>
+        <v>674</v>
       </c>
       <c r="Z54" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
-      <c r="J57" s="44"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="40"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B58" s="38"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="41" t="s">
+      <c r="B58" s="47"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="41"/>
+      <c r="L58" s="44"/>
     </row>
     <row r="59" spans="1:26" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
@@ -7553,7 +7623,7 @@
       <c r="L59" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M59" s="37" t="s">
+      <c r="M59" s="36" t="s">
         <v>20</v>
       </c>
       <c r="N59" s="11" t="s">
@@ -7754,6 +7824,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="B18:J18"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="B58:J58"/>
@@ -7765,51 +7841,58 @@
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="B57:J57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B43:J43"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B18:J18"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L15 L60:L68 L33:L41 L20:L28 L90:L1048576">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="25" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L46:L54">
-    <cfRule type="cellIs" dxfId="6" priority="14" operator="between">
-      <formula>0.5</formula>
-      <formula>0.8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="lessThan">
-      <formula>0.5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="greaterThan">
-      <formula>0.8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K15 K33:K41 K60:K1048576 K20:K29 K46:K57 K17">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="K7:K15 K33:K41 K60:K1048576 K20:K29 K55:K57 K17">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68 C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B15 C8 D9 C11:C12 D11 D13:D15 C14:C15 E15 F10:G10 F12:G15 B20:B28 C21 D22 D24 C24:C25 D26 C27:D28 F23:G23 F25:G28 E28 B33:B41 C34 D35 C37:C38 D37 C40:C41 D39:D40 D41:E41 F36:G36 F38:G41">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L54">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+      <formula>0.5</formula>
+      <formula>0.8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46:K54">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>-25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
@@ -15209,11 +15292,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1794C70D-1077-484D-B5F6-2A3A99F052C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CDD631-E1CF-4B20-90E7-7B13F37D5249}">
   <dimension ref="A1:A528"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15266,27 +15349,27 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -15325,12 +15408,12 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>653</v>
+        <v>680</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>654</v>
+        <v>681</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -15343,17 +15426,17 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>655</v>
+        <v>682</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>656</v>
+        <v>683</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>657</v>
+        <v>684</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -15368,17 +15451,17 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>658</v>
+        <v>685</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>659</v>
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>660</v>
+        <v>687</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -15409,17 +15492,17 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>80</v>
+        <v>688</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>661</v>
+        <v>689</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>662</v>
+        <v>690</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
@@ -15437,17 +15520,17 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>663</v>
+        <v>691</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>664</v>
+        <v>692</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>665</v>
+        <v>693</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -15455,7 +15538,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -15465,7 +15548,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
@@ -15475,7 +15558,7 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
@@ -15501,27 +15584,27 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
@@ -15560,17 +15643,17 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>669</v>
+        <v>694</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>670</v>
+        <v>695</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>671</v>
+        <v>696</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
@@ -15583,17 +15666,17 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>672</v>
+        <v>697</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>673</v>
+        <v>698</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>674</v>
+        <v>699</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
@@ -15608,17 +15691,17 @@
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>675</v>
+        <v>700</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>676</v>
+        <v>701</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>677</v>
+        <v>702</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
@@ -15669,17 +15752,17 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>80</v>
+        <v>688</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>678</v>
+        <v>703</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>662</v>
+        <v>690</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
@@ -15697,17 +15780,17 @@
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>679</v>
+        <v>704</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>680</v>
+        <v>705</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>681</v>
+        <v>706</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -15715,7 +15798,7 @@
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>682</v>
+        <v>652</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
@@ -15725,7 +15808,7 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>683</v>
+        <v>653</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
@@ -15735,7 +15818,7 @@
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>684</v>
+        <v>654</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
@@ -15761,27 +15844,27 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
@@ -15820,17 +15903,17 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>685</v>
+        <v>707</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>686</v>
+        <v>708</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>687</v>
+        <v>709</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
@@ -15843,17 +15926,17 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>688</v>
+        <v>710</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>689</v>
+        <v>711</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>690</v>
+        <v>712</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
@@ -15868,17 +15951,17 @@
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>691</v>
+        <v>713</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>692</v>
+        <v>714</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>693</v>
+        <v>715</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -15891,17 +15974,17 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>694</v>
+        <v>98</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>695</v>
+        <v>663</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>696</v>
+        <v>716</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
@@ -15929,17 +16012,17 @@
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>80</v>
+        <v>688</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>697</v>
+        <v>717</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>662</v>
+        <v>690</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
@@ -15957,17 +16040,17 @@
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>698</v>
+        <v>718</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>699</v>
+        <v>719</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>700</v>
+        <v>720</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
@@ -15975,7 +16058,7 @@
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>701</v>
+        <v>655</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
@@ -15985,7 +16068,7 @@
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>702</v>
+        <v>656</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
@@ -15995,7 +16078,7 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>703</v>
+        <v>657</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
@@ -16021,27 +16104,27 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
@@ -16080,22 +16163,22 @@
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>704</v>
+        <v>721</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>705</v>
+        <v>722</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>706</v>
+        <v>723</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>707</v>
+        <v>724</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
@@ -16108,17 +16191,17 @@
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>708</v>
+        <v>725</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>709</v>
+        <v>726</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>710</v>
+        <v>727</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
@@ -16133,17 +16216,17 @@
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>711</v>
+        <v>728</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>712</v>
+        <v>729</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>713</v>
+        <v>730</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
@@ -16161,17 +16244,17 @@
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>714</v>
+        <v>658</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>716</v>
+        <v>732</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
@@ -16199,17 +16282,17 @@
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
-        <v>717</v>
+        <v>733</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>662</v>
+        <v>734</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
@@ -16227,17 +16310,17 @@
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>718</v>
+        <v>735</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
-        <v>719</v>
+        <v>736</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
-        <v>720</v>
+        <v>737</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
@@ -16245,7 +16328,7 @@
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
-        <v>721</v>
+        <v>660</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
@@ -16255,7 +16338,7 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>722</v>
+        <v>661</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
@@ -16265,7 +16348,7 @@
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
-        <v>723</v>
+        <v>662</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
@@ -16291,27 +16374,27 @@
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
@@ -16350,22 +16433,22 @@
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="3" t="s">
-        <v>724</v>
+        <v>738</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="3" t="s">
-        <v>725</v>
+        <v>739</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="3" t="s">
-        <v>726</v>
+        <v>740</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="3" t="s">
-        <v>727</v>
+        <v>741</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
@@ -16378,17 +16461,17 @@
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="3" t="s">
-        <v>728</v>
+        <v>742</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="3" t="s">
-        <v>729</v>
+        <v>743</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="3" t="s">
-        <v>730</v>
+        <v>744</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
@@ -16403,17 +16486,17 @@
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="3" t="s">
-        <v>203</v>
+        <v>745</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
-        <v>731</v>
+        <v>746</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
-        <v>732</v>
+        <v>747</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
@@ -16431,17 +16514,17 @@
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
-        <v>733</v>
+        <v>748</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
-        <v>734</v>
+        <v>749</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
-        <v>735</v>
+        <v>750</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
@@ -16469,17 +16552,17 @@
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="3" t="s">
-        <v>101</v>
+        <v>688</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="3" t="s">
-        <v>736</v>
+        <v>751</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
-        <v>737</v>
+        <v>690</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
@@ -16497,17 +16580,17 @@
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="3" t="s">
-        <v>738</v>
+        <v>752</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="3" t="s">
-        <v>739</v>
+        <v>659</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="3" t="s">
-        <v>740</v>
+        <v>753</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
@@ -16515,7 +16598,7 @@
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
-        <v>741</v>
+        <v>664</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
@@ -16525,7 +16608,7 @@
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="5" t="s">
-        <v>742</v>
+        <v>665</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
@@ -16535,7 +16618,7 @@
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="4" t="s">
-        <v>743</v>
+        <v>666</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
@@ -16561,27 +16644,27 @@
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
@@ -16620,27 +16703,27 @@
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="3" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="3" t="s">
-        <v>745</v>
+        <v>755</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="3" t="s">
-        <v>746</v>
+        <v>756</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="3" t="s">
-        <v>747</v>
+        <v>757</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="3" t="s">
-        <v>748</v>
+        <v>758</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
@@ -16653,17 +16736,17 @@
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="3" t="s">
-        <v>749</v>
+        <v>759</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="3" t="s">
-        <v>750</v>
+        <v>760</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
-        <v>751</v>
+        <v>761</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
@@ -16678,17 +16761,17 @@
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="3" t="s">
-        <v>752</v>
+        <v>762</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
-        <v>753</v>
+        <v>763</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
-        <v>754</v>
+        <v>764</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
@@ -16706,22 +16789,22 @@
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="3" t="s">
-        <v>755</v>
+        <v>765</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="3" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
-        <v>757</v>
+        <v>767</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="3" t="s">
-        <v>758</v>
+        <v>732</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
@@ -16749,17 +16832,17 @@
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="3" t="s">
-        <v>80</v>
+        <v>370</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="3" t="s">
-        <v>759</v>
+        <v>768</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="3" t="s">
-        <v>662</v>
+        <v>769</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
@@ -16777,17 +16860,17 @@
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="3" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="3" t="s">
-        <v>762</v>
+        <v>772</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
@@ -16795,7 +16878,7 @@
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="4" t="s">
-        <v>763</v>
+        <v>667</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
@@ -16805,7 +16888,7 @@
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="5" t="s">
-        <v>764</v>
+        <v>668</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
@@ -16815,7 +16898,7 @@
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="4" t="s">
-        <v>765</v>
+        <v>669</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
@@ -16841,27 +16924,27 @@
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
@@ -16900,27 +16983,27 @@
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="3" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="3" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="3" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="3" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
@@ -16933,17 +17016,17 @@
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="3" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="3" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="3" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
@@ -16958,17 +17041,17 @@
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="3" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="3" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="3" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
@@ -16986,22 +17069,22 @@
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="3" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="3" t="s">
-        <v>778</v>
+        <v>785</v>
       </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="3" t="s">
-        <v>779</v>
+        <v>786</v>
       </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="3" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
@@ -17029,17 +17112,17 @@
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="3" t="s">
-        <v>101</v>
+        <v>688</v>
       </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="3" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="3" t="s">
-        <v>737</v>
+        <v>690</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
@@ -17057,17 +17140,17 @@
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="3" t="s">
-        <v>782</v>
+        <v>789</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="3" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="3" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
@@ -17075,7 +17158,7 @@
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="4" t="s">
-        <v>785</v>
+        <v>670</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
@@ -17085,7 +17168,7 @@
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="5" t="s">
-        <v>786</v>
+        <v>671</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
@@ -17095,7 +17178,7 @@
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="4" t="s">
-        <v>787</v>
+        <v>672</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
@@ -17121,27 +17204,27 @@
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
@@ -17180,32 +17263,32 @@
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" s="3" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="3" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="3" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" s="3" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="3" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="3" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
@@ -17218,17 +17301,17 @@
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="3" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" s="3" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="3" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
@@ -17243,17 +17326,17 @@
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="3" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="3" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" s="3" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
@@ -17266,32 +17349,32 @@
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" s="3" t="s">
-        <v>325</v>
+        <v>120</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="3" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="3" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" s="3" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="3" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="3" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
@@ -17319,17 +17402,17 @@
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" s="3" t="s">
-        <v>101</v>
+        <v>688</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="3" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" s="3" t="s">
-        <v>737</v>
+        <v>690</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
@@ -17347,17 +17430,17 @@
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" s="3" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" s="3" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
@@ -17365,7 +17448,7 @@
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" s="4" t="s">
-        <v>809</v>
+        <v>673</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
@@ -17375,7 +17458,7 @@
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="5" t="s">
-        <v>810</v>
+        <v>674</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
@@ -17385,7 +17468,7 @@
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
-        <v>811</v>
+        <v>675</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
@@ -17411,27 +17494,27 @@
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
-        <v>650</v>
+        <v>677</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
-        <v>651</v>
+        <v>678</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
-        <v>652</v>
+        <v>679</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
-        <v>263</v>
+        <v>460</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
@@ -17470,37 +17553,37 @@
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" s="3" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" s="3" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" s="3" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" s="3" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
@@ -17513,17 +17596,17 @@
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" s="3" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
@@ -17538,17 +17621,17 @@
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
-        <v>435</v>
+        <v>823</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" s="3" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
@@ -17566,32 +17649,32 @@
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" s="3" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" s="3" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" s="3" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" s="3" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" s="3" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" s="3" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
@@ -17619,17 +17702,17 @@
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" s="3" t="s">
-        <v>101</v>
+        <v>688</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" s="3" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" s="3" t="s">
-        <v>737</v>
+        <v>690</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
@@ -17647,17 +17730,17 @@
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" s="3" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" s="3" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" s="3" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
@@ -17674,6 +17757,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>